<commit_message>
[feature modify] mspark, 25.01.08, Change system display resolution
</commit_message>
<xml_diff>
--- a/doc/ARG24-3 개발 history.xlsx
+++ b/doc/ARG24-3 개발 history.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.174.128\samba\arg24-3\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\8. DOC\개발 노트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2068B912-0D50-4836-A30A-EFCCF9BA34EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F33810D-E71F-4537-8BC3-A4482D21B0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="6" activeTab="9" xr2:uid="{6A061CB1-0D38-4F52-AF7C-E40E05488826}"/>
   </bookViews>
@@ -26,6 +26,7 @@
     <sheet name="wifi" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="297">
   <si>
     <t>f/w download mode</t>
   </si>
@@ -1183,7 +1184,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>kernel-5.10\drivers\video\backlight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>[feature development] mspark, 24.09.24, Add Brightness driver control</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kernel-5.10\arch\arm64\boot\dts\rockchip</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1209,7 +1218,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>kernel-5.10/drivers/video/backlight</t>
+    <t>[feature modify] mspark, 25.01.08, Change system display resolution</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>device/rockchip/common/sepolicy/vendor</t>
+  </si>
+  <si>
+    <t>LogicalDisplay.java
+prazen_sys.prop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>frameworks/base/services/core/java/com/android/server/display
+device/rockchip/rk3588</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1931,8 +1954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34670CF-CD3C-443D-908D-F0DD2F2CF773}">
   <dimension ref="B2:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2399,7 +2422,7 @@
         <v>279</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>168</v>
+        <v>294</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>280</v>
@@ -2452,22 +2475,28 @@
         <v>37</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D38" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="E38" s="15" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="2:5" ht="33" x14ac:dyDescent="0.3">
       <c r="B39" s="14">
         <v>38</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
+      <c r="C39" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="14">
@@ -3585,10 +3614,10 @@
         <v>285</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F22" s="15"/>
     </row>
@@ -3600,10 +3629,10 @@
         <v>58</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>180</v>
+        <v>288</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F23" s="15"/>
     </row>

</xml_diff>